<commit_message>
Test merge language controls
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/merge_multilanguaje/asistencia_tecnica2_ok.xlsx
+++ b/formshare/tests/resources/forms/merge_multilanguaje/asistencia_tecnica2_ok.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="158">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -486,10 +486,16 @@
     <t xml:space="preserve">version</t>
   </si>
   <si>
+    <t xml:space="preserve">form_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">Formato de asistencia tecnica V2</t>
   </si>
   <si>
     <t xml:space="preserve">3 (2021-09-20 14:25:15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asistencia_tecnica2_ok</t>
   </si>
 </sst>
 </file>
@@ -589,11 +595,11 @@
   </sheetPr>
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.45"/>
@@ -1075,7 +1081,7 @@
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.33"/>
@@ -1651,13 +1657,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.56"/>
   </cols>
@@ -1672,13 +1678,19 @@
       <c r="C1" s="0" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>